<commit_message>
added monish colleges properly
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/MGIT/MGIT_placements.xlsx
+++ b/Files/college_info/all_colleges/MGIT/MGIT_placements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91703\Desktop\gitt\PYTHON PROJECT\python_project-dataset\Files\college_info\all_colleges\MGIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91703\Desktop\DATA-INFO\MGIT_INFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23E9DC4-C655-43F7-897A-98FB27A66211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DCE764-AB06-4E79-A8C1-00B20B21C19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="105">
   <si>
     <r>
       <rPr>
@@ -831,16 +831,6 @@
         <family val="2"/>
       </rPr>
       <t>Innominds</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Carlito"/>
-        <family val="2"/>
-      </rPr>
-      <t>3.25 - 4</t>
     </r>
   </si>
   <si>
@@ -1538,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114:G120"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1565,16 +1555,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1">
@@ -1596,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4">
         <v>48</v>
@@ -1610,7 +1600,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" s="4">
         <v>20.100000000000001</v>
@@ -1624,7 +1614,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="4">
         <v>20</v>
@@ -1680,7 +1670,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="4">
         <v>15</v>
@@ -1694,7 +1684,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="4">
         <v>13</v>
@@ -1722,7 +1712,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="4">
         <v>11</v>
@@ -1750,7 +1740,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="4">
         <v>8.4</v>
@@ -1918,7 +1908,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="4">
         <v>6.1</v>
@@ -2310,7 +2300,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C54" s="4">
         <v>4.5</v>
@@ -2366,7 +2356,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C58" s="4">
         <v>4.5</v>
@@ -2380,7 +2370,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59" s="4">
         <v>4.5</v>
@@ -2436,7 +2426,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C63" s="4">
         <v>4.25</v>
@@ -2646,7 +2636,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C78" s="4">
         <v>3.6</v>
@@ -2856,7 +2846,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C93" s="4">
         <v>3.5</v>
@@ -2872,8 +2862,8 @@
       <c r="B94" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C94" s="3" t="s">
-        <v>79</v>
+      <c r="C94" s="3">
+        <v>3.25</v>
       </c>
       <c r="D94" s="2">
         <v>5</v>
@@ -2940,7 +2930,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C99" s="4">
         <v>3</v>
@@ -2968,7 +2958,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C101" s="4">
         <v>3</v>
@@ -2982,7 +2972,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C102" s="4">
         <v>3</v>
@@ -3038,7 +3028,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C106" s="4">
         <v>2.76</v>
@@ -3052,7 +3042,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C107" s="4">
         <v>2.6</v>
@@ -3066,7 +3056,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C108" s="4">
         <v>2.4</v>
@@ -3094,7 +3084,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C110" s="4">
         <v>1.8</v>
@@ -3108,7 +3098,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C111" s="4">
         <v>1.8</v>
@@ -3122,7 +3112,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C112" s="4">
         <v>1.8</v>

</xml_diff>